<commit_message>
re-run FARM with HERON 731720c3, windows
</commit_message>
<xml_diff>
--- a/tests/heron_validator/ARMA/ARMA_Sine_13h/data_worksheet.xlsx
+++ b/tests/heron_validator/ARMA/ARMA_Sine_13h/data_worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\wanghy_fork\FARM\tests\heron_validator\ARMA\ARMA_Sine_13h\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D02A9C-04EE-45F8-910B-A6A26187040B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0A5D87-DA11-4717-A488-D68F9EDF5BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38385" yWindow="-1530" windowWidth="10065" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18180" yWindow="855" windowWidth="16200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -237,37 +237,37 @@
                   <c:v>-67.61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-57.21</c:v>
+                  <c:v>-57.61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-49.596671601283674</c:v>
+                  <c:v>-50.289491924311228</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-46.81</c:v>
+                  <c:v>-47.61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-49.596671601283674</c:v>
+                  <c:v>-50.289491924311221</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-57.209999999999994</c:v>
+                  <c:v>-57.609999999999992</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-67.61</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-78.009999999999991</c:v>
+                  <c:v>-77.61</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-85.623328398716325</c:v>
+                  <c:v>-84.930508075688763</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-88.41</c:v>
+                  <c:v>-87.61</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-85.623328398716325</c:v>
+                  <c:v>-84.930508075688778</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-78.010000000000005</c:v>
+                  <c:v>-77.610000000000014</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>-67.61</c:v>
@@ -1350,7 +1350,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>20.8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B5">
         <f t="shared" ref="B5:B16" si="0">-B$1+B$2*SIN(PI()/6*A5)</f>
-        <v>-57.21</v>
+        <v>-57.61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>-49.596671601283674</v>
+        <v>-50.289491924311228</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>-46.81</v>
+        <v>-47.61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>-49.596671601283674</v>
+        <v>-50.289491924311221</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>-57.209999999999994</v>
+        <v>-57.609999999999992</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>-78.009999999999991</v>
+        <v>-77.61</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>-85.623328398716325</v>
+        <v>-84.930508075688763</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>-88.41</v>
+        <v>-87.61</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>-85.623328398716325</v>
+        <v>-84.930508075688778</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>-78.010000000000005</v>
+        <v>-77.610000000000014</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>